<commit_message>
Proccess Flow adjustment. Device Names are typed into webpage textbox iteratively.
</commit_message>
<xml_diff>
--- a/Connected Office Test Data.xlsx
+++ b/Connected Office Test Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacqui.Muller\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gary\Documents\UiPath\ConnectedOfficeWebApplication_UserAcceptanceTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCAB8EEF-425E-42A8-A7F1-FF25847C778D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3022CFEE-5723-457A-B048-9472B147003E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25185" yWindow="2715" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Device" sheetId="1" r:id="rId1"/>
@@ -686,7 +686,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
@@ -1127,7 +1127,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{243FE4D3-E987-44A9-BA20-E766DD09E091}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fourth Commit. In this commit I enabled results testing for a created device, specifically "D01 create test passed" It is successful and changed the cell B16 from FALSE to TRUE.
</commit_message>
<xml_diff>
--- a/Connected Office Test Data.xlsx
+++ b/Connected Office Test Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gary\Documents\UiPath\ConnectedOfficeWebApplication_UserAcceptanceTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3022CFEE-5723-457A-B048-9472B147003E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC2CD5D0-B880-47A2-9E55-8DEEA45FB9FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25185" yWindow="2715" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2145" yWindow="2700" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Device" sheetId="1" r:id="rId1"/>
@@ -686,7 +686,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
@@ -1127,7 +1127,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{243FE4D3-E987-44A9-BA20-E766DD09E091}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -1399,7 +1399,7 @@
         <v>48</v>
       </c>
       <c r="B16" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16" s="2" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Final Commit. I have added the results record and updated the csv file to reflect true for the records I requested results for. Project is complete.
</commit_message>
<xml_diff>
--- a/Connected Office Test Data.xlsx
+++ b/Connected Office Test Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gary\Documents\UiPath\ConnectedOfficeWebApplication_UserAcceptanceTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC2CD5D0-B880-47A2-9E55-8DEEA45FB9FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{276794FC-FE82-400C-9D24-76D86449AE1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2145" yWindow="2700" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27000" yWindow="2760" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Device" sheetId="1" r:id="rId1"/>
@@ -1128,7 +1128,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1399,7 +1399,7 @@
         <v>48</v>
       </c>
       <c r="B16" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16" s="2" t="b">
         <v>0</v>
@@ -1433,7 +1433,7 @@
         <v>50</v>
       </c>
       <c r="B18" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18" s="2" t="b">
         <v>0</v>

</xml_diff>